<commit_message>
Cross Browser Testing. Parameter in testng.xml Chrome/Firefox in beforeClass
</commit_message>
<xml_diff>
--- a/Test_data/BookNew.xlsx
+++ b/Test_data/BookNew.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rida.madrane\eclipse-workspace\Selenium_PageObjectModel_DataDriven_PhpTravels\Test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558D5B15-EA29-4B2B-A232-D766A874D1FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D51A68-1F09-4E5A-9578-B655BD434DAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{EDA00C90-19E0-4D04-9E0D-17BB46BC36FB}"/>
   </bookViews>
@@ -62,16 +62,16 @@
     <t>23455</t>
   </si>
   <si>
-    <t>Yasser001@gmail.com</t>
-  </si>
-  <si>
-    <t>Yasser002@gmail.com</t>
-  </si>
-  <si>
-    <t>Yasser003@gmail.com</t>
-  </si>
-  <si>
-    <t>Yasser004@gmail.com</t>
+    <t>Yasser005@gmail.com</t>
+  </si>
+  <si>
+    <t>Yasser006@gmail.com</t>
+  </si>
+  <si>
+    <t>Yasser007@gmail.com</t>
+  </si>
+  <si>
+    <t>Yasser008@gmail.com</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
How To take Screensots. Einige Code sind auskommentiert, damit Scrrenshot funktioniert
</commit_message>
<xml_diff>
--- a/Test_data/BookNew.xlsx
+++ b/Test_data/BookNew.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rida.madrane\eclipse-workspace\Selenium_PageObjectModel_DataDriven_PhpTravels\Test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D51A68-1F09-4E5A-9578-B655BD434DAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53E83CC-C196-473D-B6DB-FFE497F96F00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{EDA00C90-19E0-4D04-9E0D-17BB46BC36FB}"/>
   </bookViews>
@@ -62,16 +62,16 @@
     <t>23455</t>
   </si>
   <si>
-    <t>Yasser005@gmail.com</t>
-  </si>
-  <si>
-    <t>Yasser006@gmail.com</t>
-  </si>
-  <si>
-    <t>Yasser007@gmail.com</t>
-  </si>
-  <si>
     <t>Yasser008@gmail.com</t>
+  </si>
+  <si>
+    <t>Yasser009@gmail.com</t>
+  </si>
+  <si>
+    <t>Yasser010@gmail.com</t>
+  </si>
+  <si>
+    <t>Yasser011s@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -499,7 +499,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
@@ -519,7 +519,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
@@ -539,7 +539,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
@@ -559,7 +559,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
PageObjectModel Final ohne ScreenshotundParallel-Implemtantion
</commit_message>
<xml_diff>
--- a/Test_data/BookNew.xlsx
+++ b/Test_data/BookNew.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rida.madrane\eclipse-workspace\Selenium_PageObjectModel_DataDriven_PhpTravels\Test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53E83CC-C196-473D-B6DB-FFE497F96F00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEA31DC-A632-4487-8405-A92AD503A64F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{EDA00C90-19E0-4D04-9E0D-17BB46BC36FB}"/>
   </bookViews>
@@ -62,16 +62,16 @@
     <t>23455</t>
   </si>
   <si>
-    <t>Yasser008@gmail.com</t>
-  </si>
-  <si>
-    <t>Yasser009@gmail.com</t>
-  </si>
-  <si>
-    <t>Yasser010@gmail.com</t>
-  </si>
-  <si>
-    <t>Yasser011s@gmail.com</t>
+    <t>Yasser025@gmail.com</t>
+  </si>
+  <si>
+    <t>Yasser026@gmail.com</t>
+  </si>
+  <si>
+    <t>Yasser027@gmail.com</t>
+  </si>
+  <si>
+    <t>Yasser028@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -499,7 +499,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
@@ -519,7 +519,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
@@ -539,7 +539,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
@@ -559,7 +559,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>7</v>

</xml_diff>